<commit_message>
enatlpía y tablas de saturacion numericas listas
</commit_message>
<xml_diff>
--- a/app/assets/tables/H134A_tsat.xlsx
+++ b/app/assets/tables/H134A_tsat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amparoquiroz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amparoquiroz/Desktop/unlockEd/app/app/assets/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E509883F-2D08-E244-8E68-28C762C1516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4150BE10-0F54-AA45-A5DE-99B41B0F1E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15640" xr2:uid="{2E5AD26A-C036-894F-A8A1-88CA691886D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="9">
   <si>
     <t>P (kPa)</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Variable</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:F361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E360" sqref="E360"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,7 +432,9 @@
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>